<commit_message>
Redeem points 79174445 30.0
</commit_message>
<xml_diff>
--- a/redemptions.xlsx
+++ b/redemptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,10 +451,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A2" t="n">
+        <v>79174445</v>
       </c>
       <c r="B2" t="n">
         <v>20</v>
@@ -462,6 +460,21 @@
       <c r="C2" t="inlineStr">
         <is>
           <t>2025-08-18T08:46:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>30</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2025-08-18T08:51:16</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Redeem points 79174445 20.0
</commit_message>
<xml_diff>
--- a/redemptions.xlsx
+++ b/redemptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,10 +464,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A3" t="n">
+        <v>79174445</v>
       </c>
       <c r="B3" t="n">
         <v>30</v>
@@ -475,6 +473,21 @@
       <c r="C3" t="inlineStr">
         <is>
           <t>2025-08-18T08:51:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>20</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-08-18T08:51:52</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Redeem points 71277628 80.0
</commit_message>
<xml_diff>
--- a/redemptions.xlsx
+++ b/redemptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,10 +516,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A7" t="n">
+        <v>79174445</v>
       </c>
       <c r="B7" t="n">
         <v>20</v>
@@ -527,6 +525,21 @@
       <c r="C7" t="inlineStr">
         <is>
           <t>2025-08-18T09:08:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>71277628</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>80</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2025-08-18T16:53:26</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Redeem points 71277628 760.0
</commit_message>
<xml_diff>
--- a/redemptions.xlsx
+++ b/redemptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,10 +529,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>71277628</t>
-        </is>
+      <c r="A8" t="n">
+        <v>71277628</v>
       </c>
       <c r="B8" t="n">
         <v>80</v>
@@ -540,6 +538,21 @@
       <c r="C8" t="inlineStr">
         <is>
           <t>2025-08-18T16:53:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>71277628</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>760</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2025-08-18T16:53:40</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Redeem points 71277628 766.0
</commit_message>
<xml_diff>
--- a/redemptions.xlsx
+++ b/redemptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -542,10 +542,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>71277628</t>
-        </is>
+      <c r="A9" t="n">
+        <v>71277628</v>
       </c>
       <c r="B9" t="n">
         <v>760</v>
@@ -553,6 +551,21 @@
       <c r="C9" t="inlineStr">
         <is>
           <t>2025-08-18T16:53:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>71277628</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>766</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2025-08-18T16:53:54</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Redeem points 71277628 76.0
</commit_message>
<xml_diff>
--- a/redemptions.xlsx
+++ b/redemptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -568,10 +568,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>71277628</t>
-        </is>
+      <c r="A11" t="n">
+        <v>71277628</v>
       </c>
       <c r="B11" t="n">
         <v>766</v>
@@ -579,6 +577,21 @@
       <c r="C11" t="inlineStr">
         <is>
           <t>2025-08-18T16:54:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>71277628</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>76</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2025-08-18T16:54:45</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Redeem points 71277620 76.0
</commit_message>
<xml_diff>
--- a/redemptions.xlsx
+++ b/redemptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -607,10 +607,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>71277628</t>
-        </is>
+      <c r="A14" t="n">
+        <v>71277628</v>
       </c>
       <c r="B14" t="n">
         <v>76</v>
@@ -618,6 +616,21 @@
       <c r="C14" t="inlineStr">
         <is>
           <t>2025-08-18T16:54:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>71277620</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>76</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:04:15</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Redeem points 71277620 760.0
</commit_message>
<xml_diff>
--- a/redemptions.xlsx
+++ b/redemptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -620,10 +620,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>71277620</t>
-        </is>
+      <c r="A15" t="n">
+        <v>71277620</v>
       </c>
       <c r="B15" t="n">
         <v>76</v>
@@ -631,6 +629,21 @@
       <c r="C15" t="inlineStr">
         <is>
           <t>2025-08-18T17:04:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>71277620</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>760</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:04:26</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Redeem points 71277620 100.0
</commit_message>
<xml_diff>
--- a/redemptions.xlsx
+++ b/redemptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -685,10 +685,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>71277620</t>
-        </is>
+      <c r="A20" t="n">
+        <v>71277620</v>
       </c>
       <c r="B20" t="n">
         <v>76</v>
@@ -696,6 +694,21 @@
       <c r="C20" t="inlineStr">
         <is>
           <t>2025-08-18T17:28:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>71277620</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>100</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:29:26</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Redeem points 79174445 100.0
</commit_message>
<xml_diff>
--- a/redemptions.xlsx
+++ b/redemptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -698,10 +698,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>71277620</t>
-        </is>
+      <c r="A21" t="n">
+        <v>71277620</v>
       </c>
       <c r="B21" t="n">
         <v>100</v>
@@ -709,6 +707,21 @@
       <c r="C21" t="inlineStr">
         <is>
           <t>2025-08-18T17:29:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>100</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:42:29</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Redeem points 79174445 500.0
</commit_message>
<xml_diff>
--- a/redemptions.xlsx
+++ b/redemptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -711,10 +711,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A22" t="n">
+        <v>79174445</v>
       </c>
       <c r="B22" t="n">
         <v>100</v>
@@ -722,6 +720,21 @@
       <c r="C22" t="inlineStr">
         <is>
           <t>2025-08-18T17:42:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>79174445</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>500</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:43:28</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Redeem points 71076783 100.0
</commit_message>
<xml_diff>
--- a/redemptions.xlsx
+++ b/redemptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -724,10 +724,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A23" t="n">
+        <v>79174445</v>
       </c>
       <c r="B23" t="n">
         <v>500</v>
@@ -735,6 +733,21 @@
       <c r="C23" t="inlineStr">
         <is>
           <t>2025-08-18T17:43:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>71076783</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>100</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2025-08-18T17:50:48</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Redeem points 76442781 100.0
</commit_message>
<xml_diff>
--- a/redemptions.xlsx
+++ b/redemptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -763,10 +763,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>71076783</t>
-        </is>
+      <c r="A26" t="n">
+        <v>71076783</v>
       </c>
       <c r="B26" t="n">
         <v>100</v>
@@ -774,6 +772,21 @@
       <c r="C26" t="inlineStr">
         <is>
           <t>2025-08-18T18:01:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>76442781</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>100</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2025-08-18T18:06:34</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Redeem points 76442781 250.0
</commit_message>
<xml_diff>
--- a/redemptions.xlsx
+++ b/redemptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -776,10 +776,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>76442781</t>
-        </is>
+      <c r="A27" t="n">
+        <v>76442781</v>
       </c>
       <c r="B27" t="n">
         <v>100</v>
@@ -787,6 +785,21 @@
       <c r="C27" t="inlineStr">
         <is>
           <t>2025-08-18T18:06:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>76442781</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>250</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2025-08-18T18:08:21</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Redeem points 51616191 100.0
</commit_message>
<xml_diff>
--- a/redemptions.xlsx
+++ b/redemptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -789,10 +789,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>76442781</t>
-        </is>
+      <c r="A28" t="n">
+        <v>76442781</v>
       </c>
       <c r="B28" t="n">
         <v>250</v>
@@ -800,6 +798,21 @@
       <c r="C28" t="inlineStr">
         <is>
           <t>2025-08-18T18:08:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>51616191</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>100</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2025-08-20T08:04:39</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Redeem points 71717173 100.0
</commit_message>
<xml_diff>
--- a/redemptions.xlsx
+++ b/redemptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -802,10 +802,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>51616191</t>
-        </is>
+      <c r="A29" t="n">
+        <v>51616191</v>
       </c>
       <c r="B29" t="n">
         <v>100</v>
@@ -813,6 +811,21 @@
       <c r="C29" t="inlineStr">
         <is>
           <t>2025-08-20T08:04:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>71717173</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>100</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2025-08-20T08:24:26</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Redeem points 76442781 500.0
</commit_message>
<xml_diff>
--- a/redemptions.xlsx
+++ b/redemptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,6 +450,21 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>76442781</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>500</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-08-20T08:55:01</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Reset redemptions.xlsx (clear all data)
</commit_message>
<xml_diff>
--- a/redemptions.xlsx
+++ b/redemptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,21 +450,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>76442781</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>500</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2025-08-20T08:55:01</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>